<commit_message>
organizational and word document changes
</commit_message>
<xml_diff>
--- a/Figures and Graphs/figures/seedling plot AICc table.xlsx
+++ b/Figures and Graphs/figures/seedling plot AICc table.xlsx
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>AICc value</t>
-  </si>
-  <si>
     <t>difference</t>
   </si>
   <si>
@@ -57,6 +51,12 @@
   </si>
   <si>
     <t>Carica papaya</t>
+  </si>
+  <si>
+    <t>Seedling species</t>
+  </si>
+  <si>
+    <t>Model AICc value</t>
   </si>
 </sst>
 </file>
@@ -100,15 +100,21 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -125,21 +131,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +499,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,90 +511,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>155.81</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>121.13</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <f>B3-C3</f>
         <v>34.680000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
         <v>100.51</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>78.39</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <f>B4-C4</f>
         <v>22.120000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>114.55</v>
+      </c>
+      <c r="C5" s="5">
+        <v>105.27</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5" si="0">B5-C5</f>
+        <v>9.2800000000000011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>114.55</v>
-      </c>
-      <c r="C5" s="1">
-        <v>105.27</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" ref="D4:D8" si="0">B5-C5</f>
-        <v>9.2800000000000011</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>94.17</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>86.4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <f>B6-C6</f>
         <v>7.769999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
+      <c r="A7" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>79.36</v>
@@ -566,21 +608,24 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="A8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
         <v>46.22</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>48.94</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <f>B8-C8</f>
         <v>-2.7199999999999989</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>